<commit_message>
adding exercise to make practise
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi.borriello2\Desktop\Tirocinio\Tiny-MachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F618E52-EAFC-4C2D-99B7-9056EAD74AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4E7B18-39D1-4EC1-B645-40D262B0F107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4369CB72-3CB2-48AE-831B-B67D7B2D2361}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Data</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Dispense Unibo / Youtube</t>
+  </si>
+  <si>
+    <t>Test sensori arduino</t>
+  </si>
+  <si>
+    <t>Arduino Doc</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,10 +538,18 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="4">
+        <v>44600</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">

</xml_diff>